<commit_message>
DB with crypto options
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zbytek\Škola\VUT\BPC-TLI3\SP-BP\micoto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AB15616-BC71-4488-ACF2-1BE63F29397B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D407618-2559-4995-92B8-CA3E9D4991A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{62C16072-9933-48D6-B3EA-B3D4A7D747CA}"/>
+    <workbookView xWindow="46008" yWindow="0" windowWidth="15432" windowHeight="16680" activeTab="1" xr2:uid="{62C16072-9933-48D6-B3EA-B3D4A7D747CA}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -54,16 +54,34 @@
   </si>
   <si>
     <t>https://pycryptodome.readthedocs.io/en/latest/src/cipher/aes.html</t>
+  </si>
+  <si>
+    <t>devUser</t>
+  </si>
+  <si>
+    <t>https://cryptography.io/en/latest/fernet/</t>
+  </si>
+  <si>
+    <t>cryptography</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -87,13 +105,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -406,35 +427,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3AF40F-B768-429B-95FD-4198CF433CC4}">
-  <dimension ref="B2:F2"/>
+  <dimension ref="B2:G2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8449C74-B5EA-4ABA-BE53-389E9CB0E50A}">
+  <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C29:C30"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -442,55 +496,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8449C74-B5EA-4ABA-BE53-389E9CB0E50A}">
-  <dimension ref="B2"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31689734-D993-413E-9D5B-46633E6A56F1}">
+  <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>5</v>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31689734-D993-413E-9D5B-46633E6A56F1}">
-  <dimension ref="B2:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{0151E176-D2D4-4ED8-BE56-F41DA4F1094A}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{BB9B65E6-BC4E-4FF6-945D-B43C63F9048C}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{AA671CE2-7D4D-4AC9-9119-2DFA6BD64E3E}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{FC64C8FD-32E1-4DAA-95AE-308053F3D170}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fernet for encryption + device adding to DB created
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zbytek\Škola\VUT\BPC-TLI3\SP-BP\micoto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D407618-2559-4995-92B8-CA3E9D4991A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7710E531-56AD-456A-AB4C-53E87F89246E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46008" yWindow="0" windowWidth="15432" windowHeight="16680" activeTab="1" xr2:uid="{62C16072-9933-48D6-B3EA-B3D4A7D747CA}"/>
+    <workbookView xWindow="30720" yWindow="0" windowWidth="15288" windowHeight="16680" xr2:uid="{62C16072-9933-48D6-B3EA-B3D4A7D747CA}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>cryptography</t>
+  </si>
+  <si>
+    <t>devPort</t>
   </si>
 </sst>
 </file>
@@ -427,22 +430,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3AF40F-B768-429B-95FD-4198CF433CC4}">
-  <dimension ref="B2:G2"/>
+  <dimension ref="B2:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="4" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -456,9 +459,12 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -472,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8449C74-B5EA-4ABA-BE53-389E9CB0E50A}">
   <dimension ref="B2:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,7 +507,7 @@
   <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Changed to AES256-CBC, start of GUI
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zbytek\Škola\VUT\BPC-TLI3\SP-BP\micoto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E288663-203F-4A63-9022-DC48C4B9BE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2872227A-5752-499A-96A5-B4BC14CC7A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="0" windowWidth="15288" windowHeight="16680" xr2:uid="{62C16072-9933-48D6-B3EA-B3D4A7D747CA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15408" windowHeight="16680" activeTab="2" xr2:uid="{62C16072-9933-48D6-B3EA-B3D4A7D747CA}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -53,9 +53,6 @@
     <t>https://help.mikrotik.com/docs/spaces/ROS/pages/47579209/Python3+Example</t>
   </si>
   <si>
-    <t>https://pycryptodome.readthedocs.io/en/latest/src/cipher/aes.html</t>
-  </si>
-  <si>
     <t>devUser</t>
   </si>
   <si>
@@ -63,6 +60,30 @@
   </si>
   <si>
     <t>cryptography</t>
+  </si>
+  <si>
+    <t>devNonce</t>
+  </si>
+  <si>
+    <t>depricated</t>
+  </si>
+  <si>
+    <t>https://cryptography.io/en/latest/hazmat/primitives/symmetric-encryption/</t>
+  </si>
+  <si>
+    <t>https://github.com/hoffstadt/DearPyGui</t>
+  </si>
+  <si>
+    <t>sqlite3</t>
+  </si>
+  <si>
+    <t>mikrotik api</t>
+  </si>
+  <si>
+    <t>crypto</t>
+  </si>
+  <si>
+    <t>gui</t>
   </si>
 </sst>
 </file>
@@ -427,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3AF40F-B768-429B-95FD-4198CF433CC4}">
-  <dimension ref="B2:G2"/>
+  <dimension ref="B2:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,7 +462,7 @@
     <col min="6" max="6" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -455,10 +476,13 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +511,7 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -497,40 +521,64 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31689734-D993-413E-9D5B-46633E6A56F1}">
-  <dimension ref="B2:B6"/>
+  <dimension ref="A2:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{0151E176-D2D4-4ED8-BE56-F41DA4F1094A}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{BB9B65E6-BC4E-4FF6-945D-B43C63F9048C}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{AA671CE2-7D4D-4AC9-9119-2DFA6BD64E3E}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{FC64C8FD-32E1-4DAA-95AE-308053F3D170}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{AA671CE2-7D4D-4AC9-9119-2DFA6BD64E3E}"/>
+    <hyperlink ref="K3" r:id="rId3" xr:uid="{02D6F45C-76BB-4A60-B476-669339D11E07}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{EC43DBF8-527A-4B01-AD43-A113531837D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rwe design redo in progress
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zbytek\Škola\VUT\BPC-TLI3\SP-BP\micoto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jirka\Desktop\micoto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB56E582-2FE7-4758-BFBD-A0D77BFE4BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1356DE1-4520-44A4-99BD-F71F75212427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{62C16072-9933-48D6-B3EA-B3D4A7D747CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{62C16072-9933-48D6-B3EA-B3D4A7D747CA}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>devName</t>
-  </si>
-  <si>
     <t>devIp</t>
   </si>
   <si>
@@ -92,15 +89,6 @@
     <t>devices</t>
   </si>
   <si>
-    <t>cammands</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>fullWord</t>
-  </si>
-  <si>
     <t>telnet</t>
   </si>
   <si>
@@ -114,13 +102,28 @@
   </si>
   <si>
     <t>dalo by se ujebat!?</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>commands</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>set</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -162,16 +165,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -488,62 +544,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3AF40F-B768-429B-95FD-4198CF433CC4}">
-  <dimension ref="B1:L2"/>
+  <dimension ref="B1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1">
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="2:12" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
+      <c r="J2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="15.75" thickTop="1">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -557,14 +647,14 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -576,90 +666,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31689734-D993-413E-9D5B-46633E6A56F1}">
   <dimension ref="A2:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="K9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="K10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11">
       <c r="K11" s="1"/>
     </row>
   </sheetData>

</xml_diff>